<commit_message>
Added: Raising query format.
</commit_message>
<xml_diff>
--- a/Production_tracker_template.xlsx
+++ b/Production_tracker_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t xml:space="preserve">Start time</t>
   </si>
@@ -101,16 +101,13 @@
     <t xml:space="preserve">NCC</t>
   </si>
   <si>
-    <t xml:space="preserve">ERP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSS SAFARICOM|| Connection Migration Failure at ERP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ConnectionMigration failure at ERP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raised to ERP for WA</t>
+    <t xml:space="preserve">BSS SAFARICOM || Provisioning Failures from NCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provisioning Order Failure at NCC for WA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raised to NCC for WA</t>
   </si>
   <si>
     <t xml:space="preserve">Priority</t>
@@ -125,23 +122,26 @@
     <t xml:space="preserve">Asnake</t>
   </si>
   <si>
-    <t xml:space="preserve">INC000000029675</t>
+    <t xml:space="preserve">INC000000030904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$N$23:$N$27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,7 +166,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -177,6 +177,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -193,12 +198,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -227,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,64 +268,56 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -499,10 +503,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -514,9 +518,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="3.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="2.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.15"/>
   </cols>
   <sheetData>
@@ -582,284 +586,276 @@
     <row r="2" customFormat="false" ht="18.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <f aca="false">B5</f>
-        <v>45337.6951388889</v>
+        <v>45339.8291666667</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10" t="str">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="str">
         <f aca="false">B7</f>
         <v>Issue</v>
       </c>
-      <c r="E2" s="10" t="str">
-        <f aca="false">B10</f>
-        <v>ERP</v>
-      </c>
-      <c r="F2" s="10" t="str">
+      <c r="E2" s="9" t="str">
+        <f aca="false">B8</f>
+        <v>By BSS</v>
+      </c>
+      <c r="F2" s="9" t="str">
         <f aca="false">B9</f>
         <v>External</v>
       </c>
-      <c r="G2" s="10" t="str">
+      <c r="G2" s="9" t="str">
         <f aca="false">B10</f>
-        <v>ERP</v>
-      </c>
-      <c r="H2" s="10" t="str">
+        <v>NCC</v>
+      </c>
+      <c r="H2" s="9" t="str">
         <f aca="false">B11</f>
-        <v>BSS SAFARICOM|| Connection Migration Failure at ERP</v>
-      </c>
-      <c r="I2" s="10" t="str">
+        <v>BSS SAFARICOM || Provisioning Failures from NCC</v>
+      </c>
+      <c r="I2" s="9" t="str">
         <f aca="false">B12</f>
-        <v>ConnectionMigration failure at ERP</v>
-      </c>
-      <c r="J2" s="10" t="str">
+        <v>Provisioning Order Failure at NCC for WA</v>
+      </c>
+      <c r="J2" s="9" t="str">
         <f aca="false">B13</f>
-        <v>Raised to ERP for WA</v>
-      </c>
-      <c r="K2" s="10" t="str">
+        <v>Raised to NCC for WA</v>
+      </c>
+      <c r="K2" s="9" t="str">
         <f aca="false">B14</f>
         <v>P4</v>
       </c>
       <c r="L2" s="8"/>
-      <c r="M2" s="10" t="str">
+      <c r="M2" s="9" t="str">
         <f aca="false">B16</f>
         <v>Open</v>
       </c>
-      <c r="N2" s="10" t="str">
+      <c r="N2" s="9" t="str">
         <f aca="false">B17</f>
         <v>Asnake</v>
       </c>
       <c r="O2" s="8"/>
-      <c r="P2" s="10" t="str">
+      <c r="P2" s="9" t="str">
         <f aca="false">B19</f>
-        <v>INC000000029675</v>
+        <v>INC000000030904</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12" t="n">
-        <v>45337.6951388889</v>
-      </c>
-      <c r="C5" s="12"/>
+      <c r="B5" s="11" t="n">
+        <v>45339.8291666667</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="14" t="str">
-        <f aca="false">D7</f>
-        <v>Issue</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="C7" s="13"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="17" t="str">
-        <f aca="false">D8</f>
-        <v>By BSS</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="14.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="17" t="str">
-        <f aca="false">D9</f>
-        <v>External</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="17" t="str">
-        <f aca="false">D10</f>
-        <v>ERP</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="17" t="str">
-        <f aca="false">H11</f>
-        <v>BSS SAFARICOM|| Connection Migration Failure at ERP</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="H11" s="18" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="str">
-        <f aca="false">H12</f>
-        <v>ConnectionMigration failure at ERP</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="H12" s="20" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" customFormat="false" ht="19.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" customFormat="false" ht="19.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="19" t="str">
-        <f aca="false">H13</f>
-        <v>Raised to ERP for WA</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="H13" s="20" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="17" t="str">
-        <f aca="false">D14</f>
-        <v>P4</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="17" t="str">
-        <f aca="false">D16</f>
-        <v>Open</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="17" t="str">
-        <f aca="false">D17</f>
-        <v>Asnake</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="15" t="s">
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="21" t="s">
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="P23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="21"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H27" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H29" s="19"/>
+      <c r="P29" s="14" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="3:3"/>
+  <mergeCells count="18">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -870,61 +866,65 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
   </mergeCells>
-  <dataValidations count="14">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B5" type="custom">
-      <formula1>NOW()</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8 B11:B14 B16" type="none">
+  <dataValidations count="15">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D8 H28" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:B10" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10:D10" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P23" type="list">
+      <formula1>"$N$23:$N$27"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7" type="list">
+      <formula1>"Issue,Service request"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8" type="list">
+      <formula1>"By BSS,To BSS"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9" type="list">
+      <formula1>"External,Internal"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10" type="list">
+      <formula1>"NCC,ERP,PRM,BSS,UMS,NMS,LMS,SND,Tibco"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11" type="list">
+      <formula1>"BSS SAFARICOM || FNF Order Failures,BSS SAFARICOM || Provisioning Failures from NCC,BSS Safaricom || Lifecyclesync Termination failure at HLR,Language update and Change SIM active failure cases,BSS Safaricom || ChangeSubscription failure at NCC,Provisioni"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12" type="list">
+      <formula1>"ChangeSim order failure at NCC for WA,Provisioning Order Failure at NCC for WA,Provisioning order failures at SND for WA,Fnf Order Failure at NCC for WA,Connection Migration Failure at NCC for WA"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13" type="list">
+      <formula1>"Raised to ERP for WA,Raised to NCC for WA,Raised to SND  for WA,Raised to Tibco  for WA"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14" type="list">
+      <formula1>"P4,P3,P2,P1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16" type="list">
+      <formula1>"Open,Closed"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B17" type="list">
+      <formula1>"Asnake,Million,Abenezer,Seid,Akshay,Greejith,Arun,Anjali,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10" type="list">
       <formula1>"NCC,ERP,PRM,BSS,UMS,NMS,LMS"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7" type="list">
-      <formula1>"Issue,Service request"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D8" type="list">
-      <formula1>"By BSS,To BSS"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D9" type="list">
-      <formula1>"External,Internal"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D14" type="list">
-      <formula1>"P4,P3,P2,P1"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D16" type="list">
-      <formula1>"Open,Closed"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D17" type="list">
-      <formula1>"Asnake"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H11" type="list">
-      <formula1>"BSS SAFARICOM || FNF Order Failures,BSS SAFARICOM || Provisioning Failures from NCC,BSS Safaricom || Lifecyclesync Termination failure at HLR,Language update and Change SIM active failure cases,BSS Safaricom || ChangeSubscription failure at NCC,BSS SAFARI"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H12" type="list">
-      <formula1>"Fnf Order failure at NCC,Provisioning order failure at NCC ,ChangeSim order failure at NCC,ConnectionMigration failure at ERP"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H13" type="list">
-      <formula1>"Raised to ERP for WA,Raised to NCC for WA,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7" type="list">
       <formula1>"BSS SAFARICOM || FNF Order Failures,BSS SAFARICOM || Provisioning Failures from NCC,BSS Safaricom || Lifecyclesync Termination failure at HLR,Language update and Change SIM active failure cases,BSS Safaricom || ChangeSubscription failure at NCC"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P29" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Üpdated: latest june 27/2024
</commit_message>
<xml_diff>
--- a/Production_tracker_template.xlsx
+++ b/Production_tracker_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t xml:space="preserve">Start time</t>
   </si>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">Raised </t>
   </si>
   <si>
-    <t xml:space="preserve">By BSS</t>
+    <t xml:space="preserve">To BSS</t>
   </si>
   <si>
     <t xml:space="preserve">Internal/External</t>
@@ -98,16 +98,19 @@
     <t xml:space="preserve">External</t>
   </si>
   <si>
+    <t xml:space="preserve">HLR</t>
+  </si>
+  <si>
     <t xml:space="preserve">NCC</t>
   </si>
   <si>
-    <t xml:space="preserve">BSS SAFARICOM || Provisioning Failures from NCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provisioning Order Failure at NCC for WA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raised to NCC for WA</t>
+    <t xml:space="preserve">Linebarring Failed Orders | HLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linebarring Failed Orders ar HLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raised to HLR for WA</t>
   </si>
   <si>
     <t xml:space="preserve">Priority</t>
@@ -122,7 +125,7 @@
     <t xml:space="preserve">Asnake</t>
   </si>
   <si>
-    <t xml:space="preserve">INC000000030904</t>
+    <t xml:space="preserve">INC000000031410</t>
   </si>
   <si>
     <t xml:space="preserve">$N$23:$N$27</t>
@@ -239,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,12 +315,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -505,8 +504,8 @@
   </sheetPr>
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -586,7 +585,7 @@
     <row r="2" customFormat="false" ht="18.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <f aca="false">B5</f>
-        <v>45339.8291666667</v>
+        <v>45365.327297963</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="7"/>
@@ -596,7 +595,7 @@
       </c>
       <c r="E2" s="9" t="str">
         <f aca="false">B8</f>
-        <v>By BSS</v>
+        <v>To BSS</v>
       </c>
       <c r="F2" s="9" t="str">
         <f aca="false">B9</f>
@@ -604,19 +603,19 @@
       </c>
       <c r="G2" s="9" t="str">
         <f aca="false">B10</f>
-        <v>NCC</v>
+        <v>HLR</v>
       </c>
       <c r="H2" s="9" t="str">
         <f aca="false">B11</f>
-        <v>BSS SAFARICOM || Provisioning Failures from NCC</v>
+        <v>Linebarring Failed Orders | HLR</v>
       </c>
       <c r="I2" s="9" t="str">
         <f aca="false">B12</f>
-        <v>Provisioning Order Failure at NCC for WA</v>
+        <v>Linebarring Failed Orders ar HLR</v>
       </c>
       <c r="J2" s="9" t="str">
         <f aca="false">B13</f>
-        <v>Raised to NCC for WA</v>
+        <v>Raised to HLR for WA</v>
       </c>
       <c r="K2" s="9" t="str">
         <f aca="false">B14</f>
@@ -634,7 +633,7 @@
       <c r="O2" s="8"/>
       <c r="P2" s="9" t="str">
         <f aca="false">B19</f>
-        <v>INC000000030904</v>
+        <v>INC000000031410</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
@@ -655,7 +654,8 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>45339.8291666667</v>
+        <f aca="true">NOW()</f>
+        <v>45365.327297963</v>
       </c>
       <c r="C5" s="11"/>
     </row>
@@ -705,7 +705,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -725,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -737,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -746,10 +746,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="13"/>
     </row>
@@ -765,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="13"/>
     </row>
@@ -774,7 +774,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="13"/>
     </row>
@@ -790,7 +790,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="18"/>
     </row>
@@ -819,7 +819,7 @@
       <c r="H23" s="1"/>
       <c r="N23" s="1"/>
       <c r="P23" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,7 +840,7 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="19"/>
+      <c r="H29" s="14"/>
       <c r="P29" s="14" t="n">
         <v>1</v>
       </c>
@@ -888,19 +888,19 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B10" type="list">
-      <formula1>"NCC,ERP,PRM,BSS,UMS,NMS,LMS,SND,Tibco"</formula1>
+      <formula1>"NCC,ERP,PRM,BSS,UMS,NMS,LMS,SND,Tibco,HLR"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B11" type="list">
-      <formula1>"BSS SAFARICOM || FNF Order Failures,BSS SAFARICOM || Provisioning Failures from NCC,BSS Safaricom || Lifecyclesync Termination failure at HLR,Language update and Change SIM active failure cases,BSS Safaricom || ChangeSubscription failure at NCC,Provisioni"</formula1>
+      <formula1>"BSS SAFARICOM || FNF Order Failures,BSS SAFARICOM || Provisioning Failures from NCC,BSS Safaricom || Lifecyclesync Termination failure at HLR,Language update and Change SIM active failure cases,BSS Safaricom || ChangeSubscription failure at NCC,BSS Safari"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12" type="list">
-      <formula1>"ChangeSim order failure at NCC for WA,Provisioning Order Failure at NCC for WA,Provisioning order failures at SND for WA,Fnf Order Failure at NCC for WA,Connection Migration Failure at NCC for WA"</formula1>
+      <formula1>"ChangeSim order failure at NCC for WA,Provisioning Order Failure at NCC for WA,Provisioning order failures at SND for WA,Fnf Order Failure at NCC for WA,Connection Migration Failure at NCC for WA,Modifying existing customer profile  at BSS for WA,clear th"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13" type="list">
-      <formula1>"Raised to ERP for WA,Raised to NCC for WA,Raised to SND  for WA,Raised to Tibco  for WA"</formula1>
+      <formula1>"Raised to ERP for WA,Raised to NCC for WA,Raised to SND  for WA,Raised to Tibco  for WA,WA at BSS,Raised to HLR for WA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B14" type="list">
@@ -912,7 +912,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B17" type="list">
-      <formula1>"Asnake,Million,Abenezer,Seid,Akshay,Greejith,Arun,Anjali,"</formula1>
+      <formula1>"Asnake,Million,Abenezer,Seid,Akshay,Greejith,Arun,Anjali,Nishmita"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C10" type="list">

</xml_diff>